<commit_message>
Conversionld and COM_FR added and Conversionlh corrected
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\Veda_TIMES_OSeMOSYS_demo1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Veda2.0_localhost_2.17.1.1\Veda\Veda_models\Demo_models\DemoS_003\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2669BAF-6166-4A17-B0B8-05831DF465F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867F6799-63D2-4A05-822B-02C5B05CDF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="21599" windowHeight="12682" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -25,20 +25,7 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -66,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="94">
   <si>
     <t>IMP*Z</t>
   </si>
@@ -299,46 +286,55 @@
     <t>year2</t>
   </si>
   <si>
+    <t>Conversionls</t>
+  </si>
+  <si>
+    <t>DaySplit</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>other_indexes</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>S1D1</t>
+  </si>
+  <si>
+    <t>S2D1</t>
+  </si>
+  <si>
+    <t>S1D2</t>
+  </si>
+  <si>
+    <t>S2D2</t>
+  </si>
+  <si>
+    <t>Cset_SET</t>
+  </si>
+  <si>
+    <t>COM_FR</t>
+  </si>
+  <si>
+    <t>Conversionlh</t>
+  </si>
+  <si>
     <t>Conversionld</t>
-  </si>
-  <si>
-    <t>Conversionls</t>
-  </si>
-  <si>
-    <t>DaySplit</t>
-  </si>
-  <si>
-    <t>attribute</t>
-  </si>
-  <si>
-    <t>other_indexes</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>S1D1</t>
-  </si>
-  <si>
-    <t>S2D1</t>
-  </si>
-  <si>
-    <t>S1D2</t>
-  </si>
-  <si>
-    <t>S2D2</t>
   </si>
 </sst>
 </file>
@@ -348,10 +344,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -406,8 +409,128 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,8 +579,181 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -502,45 +798,236 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="47">
+    <cellStyle name="20% - Accent1" xfId="22" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="26" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="30" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="34" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="38" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="42" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="23" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="27" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="31" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="35" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="39" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="43" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="24" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="28" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="32" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="36" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="40" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="44" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="21" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="25" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="29" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="33" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="37" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="41" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="11" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="15" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="17" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="19" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="10" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="9" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="13" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="16" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="12" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="45" xr:uid="{265D3D18-7C6B-434B-8C9A-7E4CD9002B9C}"/>
     <cellStyle name="Normale_B2020" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Note 2" xfId="46" xr:uid="{76B15E0F-26FB-41A8-9ECB-38E43834CA26}"/>
+    <cellStyle name="Output" xfId="14" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Standard_Sce_D_Extraction" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="20" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="18" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2378,7 +2865,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="IEA Data"/>
@@ -2833,25 +3320,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:Q23"/>
+  <dimension ref="B3:Q27"/>
   <sheetViews>
-    <sheetView topLeftCell="G5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16:P19"/>
+    <sheetView tabSelected="1" topLeftCell="G5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" customWidth="1"/>
-    <col min="2" max="2" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.59765625" customWidth="1"/>
-    <col min="8" max="8" width="29.3984375" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.73046875" customWidth="1"/>
-    <col min="17" max="17" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2861,7 +3348,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="2:17" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
@@ -2878,7 +3365,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>43</v>
       </c>
@@ -2886,42 +3373,42 @@
         <v>34</v>
       </c>
       <c r="H5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
         <v>83</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="H6" t="s">
-        <v>84</v>
-      </c>
-      <c r="J6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="N12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="N13" t="s">
+        <v>79</v>
+      </c>
+      <c r="O13" t="s">
         <v>80</v>
-      </c>
-      <c r="O13" t="s">
-        <v>81</v>
       </c>
       <c r="P13" t="s">
         <v>14</v>
       </c>
       <c r="Q13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="N14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O14">
         <v>1</v>
@@ -2931,9 +3418,9 @@
         <v>1.3698630136986301E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="N15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O15">
         <v>2</v>
@@ -2943,65 +3430,65 @@
         <v>1.3698630136986301E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="N16" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="O16">
         <v>1</v>
       </c>
       <c r="P16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="14:17" x14ac:dyDescent="0.2">
       <c r="N17" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="O17">
         <v>1</v>
       </c>
       <c r="P17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="14:17" x14ac:dyDescent="0.2">
       <c r="N18" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="O18">
         <v>2</v>
       </c>
       <c r="P18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="14:17" x14ac:dyDescent="0.2">
       <c r="N19" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="O19">
         <v>2</v>
       </c>
       <c r="P19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="14:17" x14ac:dyDescent="0.2">
       <c r="N20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O20">
         <v>1</v>
@@ -3014,9 +3501,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="14:17" x14ac:dyDescent="0.2">
       <c r="N21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O21">
         <v>2</v>
@@ -3029,9 +3516,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="14:17" x14ac:dyDescent="0.2">
       <c r="N22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O22">
         <v>1</v>
@@ -3044,9 +3531,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="14:17" x14ac:dyDescent="0.2">
       <c r="N23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O23">
         <v>2</v>
@@ -3059,8 +3546,64 @@
         <v>1</v>
       </c>
     </row>
+    <row r="24" spans="14:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>93</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="14:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>93</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="14:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>93</v>
+      </c>
+      <c r="O26">
+        <v>2</v>
+      </c>
+      <c r="P26" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="14:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="N27" t="s">
+        <v>93</v>
+      </c>
+      <c r="O27">
+        <v>2</v>
+      </c>
+      <c r="P27" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -3077,41 +3620,41 @@
       <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.86328125" customWidth="1"/>
-    <col min="3" max="3" width="29.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2005</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="12" t="s">
         <v>23</v>
       </c>
@@ -3119,7 +3662,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="13">
         <v>1</v>
       </c>
@@ -3127,7 +3670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="13">
         <v>2</v>
       </c>
@@ -3135,26 +3678,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="13"/>
       <c r="C15" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="13"/>
       <c r="C16" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="13"/>
       <c r="C17" s="13">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -3170,36 +3713,36 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.86328125" customWidth="1"/>
-    <col min="2" max="2" width="13.3984375" customWidth="1"/>
-    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.73046875" customWidth="1"/>
-    <col min="13" max="13" width="9.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="17.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:4" ht="18" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
@@ -3213,7 +3756,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -3227,7 +3770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>2</v>
       </c>
@@ -3241,12 +3784,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>16</v>
       </c>
@@ -3260,7 +3803,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>73</v>
       </c>
@@ -3285,34 +3828,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B3:G34"/>
+  <dimension ref="B3:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="9"/>
-    <col min="2" max="2" width="12.1328125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10.86328125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="9"/>
+    <col min="2" max="2" width="12.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="9" customWidth="1"/>
     <col min="4" max="4" width="14" style="9" customWidth="1"/>
-    <col min="5" max="5" width="10.3984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.3984375" style="9" customWidth="1"/>
-    <col min="7" max="16384" width="9.1328125" style="9"/>
+    <col min="5" max="5" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
@@ -3331,8 +3874,11 @@
       <c r="G6" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H6" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D7" s="9" t="s">
         <v>36</v>
       </c>
@@ -3340,7 +3886,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D8" s="9" t="s">
         <v>26</v>
       </c>
@@ -3348,7 +3894,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D9" s="9" t="s">
         <v>40</v>
       </c>
@@ -3359,9 +3905,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>35</v>
@@ -3370,9 +3916,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>35</v>
@@ -3381,9 +3927,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>35</v>
@@ -3392,9 +3938,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B13" s="20" t="s">
-        <v>90</v>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="C13"/>
       <c r="D13" s="9" t="s">
@@ -3405,107 +3951,146 @@
       </c>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B14"/>
-      <c r="C14"/>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.25</v>
+      </c>
       <c r="F14" s="15"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15"/>
-      <c r="C15"/>
+      <c r="H14" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0.25</v>
+      </c>
       <c r="F15" s="15"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17"/>
+      <c r="H15" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="9" t="s">
+        <v>89</v>
+      </c>
       <c r="C17"/>
-      <c r="D17"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D17" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
@@ -3527,13 +4112,13 @@
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
@@ -3541,7 +4126,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>29</v>
       </c>
@@ -3552,7 +4137,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
         <v>44</v>
       </c>
@@ -3563,7 +4148,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>32</v>
       </c>
@@ -3571,7 +4156,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>33</v>
       </c>
@@ -3579,12 +4164,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>47</v>
       </c>
@@ -3595,7 +4180,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>50</v>
       </c>
@@ -3606,7 +4191,7 @@
         <v>1055.55</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>51</v>
       </c>
@@ -3617,7 +4202,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>52</v>
       </c>
@@ -3628,7 +4213,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>54</v>
       </c>
@@ -3639,7 +4224,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>56</v>
       </c>
@@ -3650,7 +4235,7 @@
         <v>1.05555</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>57</v>
       </c>
@@ -3661,7 +4246,7 @@
         <v>4.1868000000000002E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>58</v>
       </c>
@@ -3672,7 +4257,7 @@
         <v>41.868000000000002</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>59</v>
       </c>
@@ -3683,7 +4268,7 @@
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>60</v>
       </c>
@@ -3694,7 +4279,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>61</v>
       </c>
@@ -3705,7 +4290,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>63</v>
       </c>
@@ -3716,7 +4301,7 @@
         <v>0.15384600000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>65</v>
       </c>
@@ -3727,7 +4312,7 @@
         <v>-1E-3</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>67</v>
       </c>
@@ -3738,7 +4323,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>68</v>
       </c>
@@ -3749,7 +4334,7 @@
         <v>37.681199999999997</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>69</v>
       </c>
@@ -3760,7 +4345,7 @@
         <v>2299</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>70</v>
       </c>
@@ -3771,7 +4356,7 @@
         <v>2.7777769999999999</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>71</v>
       </c>
@@ -3782,7 +4367,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>37</v>
       </c>

</xml_diff>